<commit_message>
Updated BPA Translator to point to correct varaiables
</commit_message>
<xml_diff>
--- a/Test_Quote.xlsx
+++ b/Test_Quote.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jowino\Documents\UiPath\VLookup Data Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF79C6F-C268-43D2-B08F-35B7B9A2311D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409809F4-7A2B-4377-97F0-F8704961F933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{BD57DB04-2CAC-4324-8C2F-19EA2F7D9A31}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="5" xr2:uid="{BD57DB04-2CAC-4324-8C2F-19EA2F7D9A31}"/>
   </bookViews>
   <sheets>
     <sheet name="BPADetails" sheetId="6" r:id="rId1"/>
@@ -3299,10 +3299,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA7D0387-9D33-42A7-95B3-3BA9813FB715}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3717,6 +3717,9 @@
         <v>243</v>
       </c>
     </row>
+    <row r="28" spans="1:6" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="33" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="34" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3759,7 +3762,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Corrected augemnets to pass data across three workflows
</commit_message>
<xml_diff>
--- a/Test_Quote.xlsx
+++ b/Test_Quote.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jowino\Documents\UiPath\VLookup Data Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66174E3-A7C0-4497-81CF-26D36CFDF62B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B8C541-1FB2-4DC4-8C5E-518864A7F467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="0" activeTab="2" xr2:uid="{BD57DB04-2CAC-4324-8C2F-19EA2F7D9A31}"/>
+    <x:workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="0" activeTab="3" xr2:uid="{BD57DB04-2CAC-4324-8C2F-19EA2F7D9A31}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="BPADetails" sheetId="6" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="300">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="294">
   <x:si>
     <x:t>Partner</x:t>
   </x:si>
@@ -888,27 +888,18 @@
     <x:t>54,000.00</x:t>
   </x:si>
   <x:si>
-    <x:t>Pole Tang S Data Table - UiPath St...</x:t>
-  </x:si>
-  <x:si>
     <x:t>1,800.00</x:t>
   </x:si>
   <x:si>
     <x:t>5</x:t>
   </x:si>
   <x:si>
-    <x:t>VLookup Pole, Supp</x:t>
-  </x:si>
-  <x:si>
     <x:t>11,000.00</x:t>
   </x:si>
   <x:si>
     <x:t>55,000.00</x:t>
   </x:si>
   <x:si>
-    <x:t>Supply and Con-as</x:t>
-  </x:si>
-  <x:si>
     <x:t>1,250.00</x:t>
   </x:si>
   <x:si>
@@ -918,9 +909,6 @@
     <x:t>7,500.00</x:t>
   </x:si>
   <x:si>
-    <x:t>Pole Tensi</x:t>
-  </x:si>
-  <x:si>
     <x:t>2,300.00</x:t>
   </x:si>
   <x:si>
@@ -930,16 +918,10 @@
     <x:t>27,600.00</x:t>
   </x:si>
   <x:si>
-    <x:t>ISP Buildir</x:t>
-  </x:si>
-  <x:si>
     <x:t>880.00</x:t>
   </x:si>
   <x:si>
     <x:t>30,800.00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Splicing, T</x:t>
   </x:si>
   <x:si>
     <x:t>440.00</x:t>
@@ -3488,8 +3470,8 @@
   </x:sheetPr>
   <x:dimension ref="A1:I34"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="A18" sqref="A18 A17:A18"/>
+    <x:sheetView workbookViewId="0">
+      <x:selection activeCell="A1" sqref="A1 1:1048576"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.726562" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3506,7 +3488,7 @@
     <x:col min="10" max="16384" width="8.726562" style="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="1" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A1" s="15" t="s">
         <x:v>251</x:v>
       </x:c>
@@ -3535,7 +3517,7 @@
         <x:v>4</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="2" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A2" s="2" t="s">
         <x:v>93</x:v>
       </x:c>
@@ -3564,7 +3546,7 @@
         <x:v>8</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="3" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A3" s="2" t="s">
         <x:v>135</x:v>
       </x:c>
@@ -3593,7 +3575,7 @@
         <x:v>8</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="4" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A4" s="2" t="s">
         <x:v>71</x:v>
       </x:c>
@@ -3622,7 +3604,7 @@
         <x:v>8</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="5" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A5" s="2" t="s">
         <x:v>76</x:v>
       </x:c>
@@ -3651,7 +3633,7 @@
         <x:v>8</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="6" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A6" s="2" t="s">
         <x:v>98</x:v>
       </x:c>
@@ -3680,7 +3662,7 @@
         <x:v>8</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="7" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A7" s="2" t="s">
         <x:v>174</x:v>
       </x:c>
@@ -3709,7 +3691,7 @@
         <x:v>8</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:10" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="8" spans="1:9" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A8" s="1" t="s">
         <x:v>158</x:v>
       </x:c>
@@ -3738,7 +3720,7 @@
         <x:v>8</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="9" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A9" s="1" t="s">
         <x:v>217</x:v>
       </x:c>
@@ -3767,7 +3749,7 @@
         <x:v>8</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="10" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A10" s="1" t="s">
         <x:v>230</x:v>
       </x:c>
@@ -3796,22 +3778,25 @@
         <x:v>8</x:v>
       </x:c>
     </x:row>
-    <x:row r="11" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="11" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A11" s="1" t="s">
-        <x:v>281</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="B11" s="1" t="s">
         <x:v>260</x:v>
       </x:c>
       <x:c r="C11" s="7" t="s">
+        <x:v>281</x:v>
+      </x:c>
+      <x:c r="D11" s="1" t="s">
         <x:v>282</x:v>
-      </x:c>
-      <x:c r="D11" s="1" t="s">
-        <x:v>283</x:v>
       </x:c>
       <x:c r="E11" s="7" t="s">
         <x:v>276</x:v>
       </x:c>
+      <x:c r="F11" s="1" t="s">
+        <x:v>163</x:v>
+      </x:c>
       <x:c r="G11" s="1" t="s">
         <x:v>6</x:v>
       </x:c>
@@ -3822,21 +3807,24 @@
         <x:v>8</x:v>
       </x:c>
     </x:row>
-    <x:row r="12" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="12" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A12" s="1" t="s">
-        <x:v>284</x:v>
+        <x:v>226</x:v>
       </x:c>
       <x:c r="B12" s="1" t="s">
         <x:v>260</x:v>
       </x:c>
       <x:c r="C12" s="12" t="s">
-        <x:v>285</x:v>
+        <x:v>283</x:v>
       </x:c>
       <x:c r="D12" s="1" t="s">
-        <x:v>283</x:v>
+        <x:v>282</x:v>
       </x:c>
       <x:c r="E12" s="12" t="s">
-        <x:v>286</x:v>
+        <x:v>284</x:v>
+      </x:c>
+      <x:c r="F12" s="1" t="s">
+        <x:v>225</x:v>
       </x:c>
       <x:c r="G12" s="1" t="s">
         <x:v>6</x:v>
@@ -3848,21 +3836,24 @@
         <x:v>8</x:v>
       </x:c>
     </x:row>
-    <x:row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <x:row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <x:c r="A13" s="1" t="s">
-        <x:v>287</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="B13" s="1" t="s">
         <x:v>260</x:v>
       </x:c>
       <x:c r="C13" s="12" t="s">
-        <x:v>288</x:v>
+        <x:v>285</x:v>
       </x:c>
       <x:c r="D13" s="1" t="s">
-        <x:v>289</x:v>
+        <x:v>286</x:v>
       </x:c>
       <x:c r="E13" s="12" t="s">
-        <x:v>290</x:v>
+        <x:v>287</x:v>
+      </x:c>
+      <x:c r="F13" s="1" t="s">
+        <x:v>154</x:v>
       </x:c>
       <x:c r="G13" s="1" t="s">
         <x:v>6</x:v>
@@ -3874,21 +3865,24 @@
         <x:v>8</x:v>
       </x:c>
     </x:row>
-    <x:row r="14" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="14" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A14" s="1" t="s">
-        <x:v>291</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="B14" s="1" t="s">
         <x:v>260</x:v>
       </x:c>
       <x:c r="C14" s="7" t="s">
-        <x:v>292</x:v>
+        <x:v>288</x:v>
       </x:c>
       <x:c r="D14" s="1" t="s">
-        <x:v>293</x:v>
+        <x:v>289</x:v>
       </x:c>
       <x:c r="E14" s="7" t="s">
-        <x:v>294</x:v>
+        <x:v>290</x:v>
+      </x:c>
+      <x:c r="F14" s="1" t="s">
+        <x:v>175</x:v>
       </x:c>
       <x:c r="G14" s="1" t="s">
         <x:v>6</x:v>
@@ -3900,21 +3894,24 @@
         <x:v>8</x:v>
       </x:c>
     </x:row>
-    <x:row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <x:row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <x:c r="A15" s="1" t="s">
-        <x:v>295</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="B15" s="1" t="s">
         <x:v>260</x:v>
       </x:c>
       <x:c r="C15" s="12" t="s">
-        <x:v>296</x:v>
+        <x:v>291</x:v>
       </x:c>
       <x:c r="D15" s="1" t="s">
         <x:v>262</x:v>
       </x:c>
       <x:c r="E15" s="12" t="s">
-        <x:v>296</x:v>
+        <x:v>291</x:v>
+      </x:c>
+      <x:c r="F15" s="1" t="s">
+        <x:v>143</x:v>
       </x:c>
       <x:c r="G15" s="1" t="s">
         <x:v>6</x:v>
@@ -3926,9 +3923,9 @@
         <x:v>8</x:v>
       </x:c>
     </x:row>
-    <x:row r="16" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="16" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A16" s="1" t="s">
-        <x:v>295</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="B16" s="1" t="s">
         <x:v>260</x:v>
@@ -3942,6 +3939,9 @@
       <x:c r="E16" s="7" t="s">
         <x:v>272</x:v>
       </x:c>
+      <x:c r="F16" s="1" t="s">
+        <x:v>201</x:v>
+      </x:c>
       <x:c r="G16" s="1" t="s">
         <x:v>6</x:v>
       </x:c>
@@ -3952,21 +3952,24 @@
         <x:v>8</x:v>
       </x:c>
     </x:row>
-    <x:row r="17" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="17" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A17" s="1" t="s">
-        <x:v>295</x:v>
+        <x:v>244</x:v>
       </x:c>
       <x:c r="B17" s="1" t="s">
         <x:v>260</x:v>
       </x:c>
       <x:c r="C17" s="12" t="s">
-        <x:v>297</x:v>
+        <x:v>292</x:v>
       </x:c>
       <x:c r="D17" s="1" t="s">
         <x:v>262</x:v>
       </x:c>
       <x:c r="E17" s="12" t="s">
-        <x:v>297</x:v>
+        <x:v>292</x:v>
+      </x:c>
+      <x:c r="F17" s="1" t="s">
+        <x:v>243</x:v>
       </x:c>
       <x:c r="G17" s="1" t="s">
         <x:v>6</x:v>
@@ -3978,45 +3981,46 @@
         <x:v>8</x:v>
       </x:c>
     </x:row>
-    <x:row r="18" spans="1:10" s="0" customFormat="1">
-      <x:c r="A18" s="0" t="s">
-        <x:v>298</x:v>
-      </x:c>
-      <x:c r="B18" s="0" t="s">
+    <x:row r="18" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <x:c r="A18" s="1" t="s">
+        <x:v>129</x:v>
+      </x:c>
+      <x:c r="B18" s="1" t="s">
         <x:v>260</x:v>
       </x:c>
-      <x:c r="C18" s="0" t="s">
-        <x:v>299</x:v>
-      </x:c>
-      <x:c r="D18" s="0" t="s">
+      <x:c r="C18" s="1" t="s">
+        <x:v>293</x:v>
+      </x:c>
+      <x:c r="D18" s="1" t="s">
         <x:v>271</x:v>
       </x:c>
-      <x:c r="E18" s="0" t="s">
-        <x:v>296</x:v>
-      </x:c>
-      <x:c r="F18" s="0" t="s"/>
-      <x:c r="G18" s="0" t="s">
+      <x:c r="E18" s="1" t="s">
+        <x:v>291</x:v>
+      </x:c>
+      <x:c r="F18" s="1" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="G18" s="1" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="H18" s="0" t="s">
+      <x:c r="H18" s="1" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="I18" s="0" t="s">
+      <x:c r="I18" s="1" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="J18" s="0" t="s"/>
-    </x:row>
-    <x:row r="19" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    </x:row>
+    <x:row r="19" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="C19" s="7" t="s"/>
       <x:c r="E19" s="7" t="s"/>
     </x:row>
-    <x:row r="20" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="20" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="C20" s="7" t="s"/>
       <x:c r="E20" s="7" t="s"/>
     </x:row>
-    <x:row r="28" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <x:row r="33" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <x:row r="34" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <x:row r="28" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <x:row r="33" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <x:row r="34" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4033,8 +4037,8 @@
   </x:sheetPr>
   <x:dimension ref="E2"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0">
-      <x:selection activeCell="B10" sqref="B10"/>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="A10" sqref="A10"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4343,20 +4347,23 @@
     </x:row>
     <x:row r="11" spans="1:13">
       <x:c r="A11" s="0" t="s">
-        <x:v>281</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
         <x:v>260</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
+        <x:v>281</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
         <x:v>282</x:v>
-      </x:c>
-      <x:c r="D11" s="0" t="s">
-        <x:v>283</x:v>
       </x:c>
       <x:c r="E11" s="0" t="s">
         <x:v>276</x:v>
       </x:c>
+      <x:c r="F11" s="0" t="s">
+        <x:v>163</x:v>
+      </x:c>
       <x:c r="G11" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
@@ -4369,19 +4376,22 @@
     </x:row>
     <x:row r="12" spans="1:13">
       <x:c r="A12" s="0" t="s">
-        <x:v>284</x:v>
+        <x:v>226</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
         <x:v>260</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>285</x:v>
+        <x:v>283</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>283</x:v>
+        <x:v>282</x:v>
       </x:c>
       <x:c r="E12" s="0" t="s">
-        <x:v>286</x:v>
+        <x:v>284</x:v>
+      </x:c>
+      <x:c r="F12" s="0" t="s">
+        <x:v>225</x:v>
       </x:c>
       <x:c r="G12" s="0" t="s">
         <x:v>6</x:v>
@@ -4395,19 +4405,22 @@
     </x:row>
     <x:row r="13" spans="1:13">
       <x:c r="A13" s="0" t="s">
-        <x:v>287</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
         <x:v>260</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>288</x:v>
+        <x:v>285</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
-        <x:v>289</x:v>
+        <x:v>286</x:v>
       </x:c>
       <x:c r="E13" s="0" t="s">
-        <x:v>290</x:v>
+        <x:v>287</x:v>
+      </x:c>
+      <x:c r="F13" s="0" t="s">
+        <x:v>154</x:v>
       </x:c>
       <x:c r="G13" s="0" t="s">
         <x:v>6</x:v>
@@ -4421,19 +4434,22 @@
     </x:row>
     <x:row r="14" spans="1:13">
       <x:c r="A14" s="0" t="s">
-        <x:v>291</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
         <x:v>260</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
-        <x:v>292</x:v>
+        <x:v>288</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
-        <x:v>293</x:v>
+        <x:v>289</x:v>
       </x:c>
       <x:c r="E14" s="0" t="s">
-        <x:v>294</x:v>
+        <x:v>290</x:v>
+      </x:c>
+      <x:c r="F14" s="0" t="s">
+        <x:v>175</x:v>
       </x:c>
       <x:c r="G14" s="0" t="s">
         <x:v>6</x:v>
@@ -4447,19 +4463,22 @@
     </x:row>
     <x:row r="15" spans="1:13">
       <x:c r="A15" s="0" t="s">
-        <x:v>295</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
         <x:v>260</x:v>
       </x:c>
       <x:c r="C15" s="0" t="s">
-        <x:v>296</x:v>
+        <x:v>291</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
         <x:v>262</x:v>
       </x:c>
       <x:c r="E15" s="0" t="s">
-        <x:v>296</x:v>
+        <x:v>291</x:v>
+      </x:c>
+      <x:c r="F15" s="0" t="s">
+        <x:v>143</x:v>
       </x:c>
       <x:c r="G15" s="0" t="s">
         <x:v>6</x:v>
@@ -4473,7 +4492,7 @@
     </x:row>
     <x:row r="16" spans="1:13">
       <x:c r="A16" s="0" t="s">
-        <x:v>295</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
         <x:v>260</x:v>
@@ -4487,6 +4506,9 @@
       <x:c r="E16" s="0" t="s">
         <x:v>272</x:v>
       </x:c>
+      <x:c r="F16" s="0" t="s">
+        <x:v>201</x:v>
+      </x:c>
       <x:c r="G16" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
@@ -4499,19 +4521,22 @@
     </x:row>
     <x:row r="17" spans="1:13">
       <x:c r="A17" s="0" t="s">
-        <x:v>295</x:v>
+        <x:v>244</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
         <x:v>260</x:v>
       </x:c>
       <x:c r="C17" s="0" t="s">
-        <x:v>297</x:v>
+        <x:v>292</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
         <x:v>262</x:v>
       </x:c>
       <x:c r="E17" s="0" t="s">
-        <x:v>297</x:v>
+        <x:v>292</x:v>
+      </x:c>
+      <x:c r="F17" s="0" t="s">
+        <x:v>243</x:v>
       </x:c>
       <x:c r="G17" s="0" t="s">
         <x:v>6</x:v>
@@ -4525,19 +4550,22 @@
     </x:row>
     <x:row r="18" spans="1:13">
       <x:c r="A18" s="0" t="s">
-        <x:v>298</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
         <x:v>260</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
-        <x:v>299</x:v>
+        <x:v>293</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
         <x:v>271</x:v>
       </x:c>
       <x:c r="E18" s="0" t="s">
-        <x:v>296</x:v>
+        <x:v>291</x:v>
+      </x:c>
+      <x:c r="F18" s="0" t="s">
+        <x:v>128</x:v>
       </x:c>
       <x:c r="G18" s="0" t="s">
         <x:v>6</x:v>

</xml_diff>

<commit_message>
Add mouse scrolls to navigate through pages to equired elements
</commit_message>
<xml_diff>
--- a/Test_Quote.xlsx
+++ b/Test_Quote.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jowino\Documents\UiPath\VLookup Data Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{387040D2-9B7C-44FB-9F00-67AF4FA092D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE52348-2E9D-4713-8409-D483DF1FE9D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
     <x:workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="0" activeTab="2" xr2:uid="{BD57DB04-2CAC-4324-8C2F-19EA2F7D9A31}"/>
   </x:bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="293">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="294">
   <x:si>
     <x:t>Partner</x:t>
   </x:si>
@@ -808,6 +808,9 @@
   </x:si>
   <x:si>
     <x:t>Total</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Oracle Description</x:t>
   </x:si>
   <x:si>
     <x:t>m</x:t>
@@ -3465,10 +3468,10 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E34"/>
+  <x:dimension ref="A1:I34"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="A1" sqref="A1 1:1048576"/>
+      <x:selection activeCell="A9" sqref="A9"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.726562" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3485,7 +3488,7 @@
     <x:col min="10" max="16384" width="8.726562" style="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="1" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A1" s="15" t="s">
         <x:v>251</x:v>
       </x:c>
@@ -3501,307 +3504,523 @@
       <x:c r="E1" s="1" t="s">
         <x:v>254</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <x:c r="F1" s="1" t="s">
+        <x:v>255</x:v>
+      </x:c>
+      <x:c r="G1" s="1" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="H1" s="1" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="I1" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A2" s="2" t="s">
         <x:v>93</x:v>
       </x:c>
       <x:c r="B2" s="3" t="s">
-        <x:v>255</x:v>
+        <x:v>256</x:v>
       </x:c>
       <x:c r="C2" s="4" t="s">
-        <x:v>256</x:v>
+        <x:v>257</x:v>
       </x:c>
       <x:c r="D2" s="5" t="s">
-        <x:v>257</x:v>
+        <x:v>258</x:v>
       </x:c>
       <x:c r="E2" s="4" t="s">
-        <x:v>258</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <x:v>259</x:v>
+      </x:c>
+      <x:c r="F2" s="1" t="s">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="G2" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H2" s="1" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I2" s="1" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A3" s="2" t="s">
         <x:v>135</x:v>
       </x:c>
       <x:c r="B3" s="3" t="s">
-        <x:v>259</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C3" s="4" t="s">
-        <x:v>260</x:v>
+        <x:v>261</x:v>
       </x:c>
       <x:c r="D3" s="5" t="s">
+        <x:v>262</x:v>
+      </x:c>
+      <x:c r="E3" s="1" t="s">
         <x:v>261</x:v>
       </x:c>
-      <x:c r="E3" s="1" t="s">
-        <x:v>260</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <x:c r="F3" s="1" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="G3" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H3" s="1" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I3" s="1" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A4" s="2" t="s">
         <x:v>71</x:v>
       </x:c>
       <x:c r="B4" s="3" t="s">
-        <x:v>255</x:v>
+        <x:v>256</x:v>
       </x:c>
       <x:c r="C4" s="4" t="s">
-        <x:v>262</x:v>
+        <x:v>263</x:v>
       </x:c>
       <x:c r="D4" s="5" t="s">
-        <x:v>263</x:v>
+        <x:v>264</x:v>
       </x:c>
       <x:c r="E4" s="12" t="s">
-        <x:v>264</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <x:v>265</x:v>
+      </x:c>
+      <x:c r="F4" s="1" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="G4" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H4" s="1" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I4" s="1" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A5" s="2" t="s">
         <x:v>76</x:v>
       </x:c>
       <x:c r="B5" s="3" t="s">
-        <x:v>255</x:v>
+        <x:v>256</x:v>
       </x:c>
       <x:c r="C5" s="4" t="s">
-        <x:v>265</x:v>
+        <x:v>266</x:v>
       </x:c>
       <x:c r="D5" s="5" t="s">
-        <x:v>263</x:v>
+        <x:v>264</x:v>
       </x:c>
       <x:c r="E5" s="1" t="s">
-        <x:v>266</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <x:v>267</x:v>
+      </x:c>
+      <x:c r="F5" s="1" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="G5" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H5" s="1" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I5" s="1" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A6" s="2" t="s">
         <x:v>98</x:v>
       </x:c>
       <x:c r="B6" s="3" t="s">
-        <x:v>255</x:v>
+        <x:v>256</x:v>
       </x:c>
       <x:c r="C6" s="4" t="s">
-        <x:v>267</x:v>
+        <x:v>268</x:v>
       </x:c>
       <x:c r="D6" s="5" t="s">
-        <x:v>263</x:v>
+        <x:v>264</x:v>
       </x:c>
       <x:c r="E6" s="1" t="s">
-        <x:v>268</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <x:v>269</x:v>
+      </x:c>
+      <x:c r="F6" s="1" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="G6" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H6" s="1" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I6" s="1" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A7" s="2" t="s">
         <x:v>174</x:v>
       </x:c>
       <x:c r="B7" s="6" t="s">
-        <x:v>259</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C7" s="4" t="s">
-        <x:v>269</x:v>
+        <x:v>270</x:v>
       </x:c>
       <x:c r="D7" s="4" t="s">
-        <x:v>270</x:v>
+        <x:v>271</x:v>
       </x:c>
       <x:c r="E7" s="12" t="s">
-        <x:v>271</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:10" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
+        <x:v>272</x:v>
+      </x:c>
+      <x:c r="F7" s="1" t="s">
+        <x:v>173</x:v>
+      </x:c>
+      <x:c r="G7" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H7" s="1" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I7" s="1" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:9" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A8" s="1" t="s">
         <x:v>158</x:v>
       </x:c>
       <x:c r="B8" s="1" t="s">
-        <x:v>259</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C8" s="1" t="s">
-        <x:v>272</x:v>
+        <x:v>273</x:v>
       </x:c>
       <x:c r="D8" s="1" t="s">
-        <x:v>273</x:v>
+        <x:v>274</x:v>
       </x:c>
       <x:c r="E8" s="12" t="s">
-        <x:v>274</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <x:v>275</x:v>
+      </x:c>
+      <x:c r="F8" s="1" t="s">
+        <x:v>157</x:v>
+      </x:c>
+      <x:c r="G8" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H8" s="1" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I8" s="1" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A9" s="1" t="s">
         <x:v>217</x:v>
       </x:c>
       <x:c r="B9" s="1" t="s">
-        <x:v>259</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C9" s="1" t="s">
-        <x:v>275</x:v>
+        <x:v>276</x:v>
       </x:c>
       <x:c r="D9" s="1" t="s">
-        <x:v>273</x:v>
+        <x:v>274</x:v>
       </x:c>
       <x:c r="E9" s="7" t="s">
-        <x:v>276</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <x:v>277</x:v>
+      </x:c>
+      <x:c r="F9" s="1" t="s">
+        <x:v>216</x:v>
+      </x:c>
+      <x:c r="G9" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H9" s="1" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I9" s="1" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A10" s="1" t="s">
         <x:v>230</x:v>
       </x:c>
       <x:c r="B10" s="1" t="s">
-        <x:v>259</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C10" s="12" t="s">
-        <x:v>277</x:v>
+        <x:v>278</x:v>
       </x:c>
       <x:c r="D10" s="1" t="s">
-        <x:v>278</x:v>
+        <x:v>279</x:v>
       </x:c>
       <x:c r="E10" s="12" t="s">
-        <x:v>279</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <x:v>280</x:v>
+      </x:c>
+      <x:c r="F10" s="1" t="s">
+        <x:v>229</x:v>
+      </x:c>
+      <x:c r="G10" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H10" s="1" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I10" s="1" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A11" s="1" t="s">
         <x:v>164</x:v>
       </x:c>
       <x:c r="B11" s="1" t="s">
-        <x:v>259</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C11" s="7" t="s">
-        <x:v>280</x:v>
+        <x:v>281</x:v>
       </x:c>
       <x:c r="D11" s="1" t="s">
-        <x:v>281</x:v>
+        <x:v>282</x:v>
       </x:c>
       <x:c r="E11" s="7" t="s">
-        <x:v>275</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <x:v>276</x:v>
+      </x:c>
+      <x:c r="F11" s="1" t="s">
+        <x:v>163</x:v>
+      </x:c>
+      <x:c r="G11" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H11" s="1" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I11" s="1" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A12" s="1" t="s">
         <x:v>226</x:v>
       </x:c>
       <x:c r="B12" s="1" t="s">
-        <x:v>259</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C12" s="12" t="s">
+        <x:v>283</x:v>
+      </x:c>
+      <x:c r="D12" s="1" t="s">
         <x:v>282</x:v>
       </x:c>
-      <x:c r="D12" s="1" t="s">
-        <x:v>281</x:v>
-      </x:c>
       <x:c r="E12" s="12" t="s">
-        <x:v>283</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <x:v>284</x:v>
+      </x:c>
+      <x:c r="F12" s="1" t="s">
+        <x:v>225</x:v>
+      </x:c>
+      <x:c r="G12" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H12" s="1" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I12" s="1" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <x:c r="A13" s="1" t="s">
         <x:v>155</x:v>
       </x:c>
       <x:c r="B13" s="1" t="s">
-        <x:v>259</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C13" s="12" t="s">
-        <x:v>284</x:v>
+        <x:v>285</x:v>
       </x:c>
       <x:c r="D13" s="1" t="s">
-        <x:v>285</x:v>
+        <x:v>286</x:v>
       </x:c>
       <x:c r="E13" s="12" t="s">
-        <x:v>286</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <x:v>287</x:v>
+      </x:c>
+      <x:c r="F13" s="1" t="s">
+        <x:v>154</x:v>
+      </x:c>
+      <x:c r="G13" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H13" s="1" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I13" s="1" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A14" s="1" t="s">
         <x:v>176</x:v>
       </x:c>
       <x:c r="B14" s="1" t="s">
-        <x:v>259</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C14" s="7" t="s">
-        <x:v>287</x:v>
+        <x:v>288</x:v>
       </x:c>
       <x:c r="D14" s="1" t="s">
-        <x:v>288</x:v>
+        <x:v>289</x:v>
       </x:c>
       <x:c r="E14" s="7" t="s">
-        <x:v>289</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <x:v>290</x:v>
+      </x:c>
+      <x:c r="F14" s="1" t="s">
+        <x:v>175</x:v>
+      </x:c>
+      <x:c r="G14" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H14" s="1" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I14" s="1" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <x:c r="A15" s="1" t="s">
         <x:v>144</x:v>
       </x:c>
       <x:c r="B15" s="1" t="s">
-        <x:v>259</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C15" s="12" t="s">
-        <x:v>290</x:v>
+        <x:v>291</x:v>
       </x:c>
       <x:c r="D15" s="1" t="s">
-        <x:v>261</x:v>
+        <x:v>262</x:v>
       </x:c>
       <x:c r="E15" s="12" t="s">
-        <x:v>290</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <x:v>291</x:v>
+      </x:c>
+      <x:c r="F15" s="1" t="s">
+        <x:v>143</x:v>
+      </x:c>
+      <x:c r="G15" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H15" s="1" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I15" s="1" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A16" s="1" t="s">
         <x:v>202</x:v>
       </x:c>
       <x:c r="B16" s="1" t="s">
-        <x:v>259</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C16" s="7" t="s">
-        <x:v>271</x:v>
+        <x:v>272</x:v>
       </x:c>
       <x:c r="D16" s="1" t="s">
-        <x:v>261</x:v>
+        <x:v>262</x:v>
       </x:c>
       <x:c r="E16" s="7" t="s">
-        <x:v>271</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <x:v>272</x:v>
+      </x:c>
+      <x:c r="F16" s="1" t="s">
+        <x:v>201</x:v>
+      </x:c>
+      <x:c r="G16" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H16" s="1" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I16" s="1" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A17" s="1" t="s">
         <x:v>244</x:v>
       </x:c>
       <x:c r="B17" s="1" t="s">
-        <x:v>259</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C17" s="12" t="s">
-        <x:v>291</x:v>
+        <x:v>292</x:v>
       </x:c>
       <x:c r="D17" s="1" t="s">
-        <x:v>261</x:v>
+        <x:v>262</x:v>
       </x:c>
       <x:c r="E17" s="12" t="s">
-        <x:v>291</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <x:v>292</x:v>
+      </x:c>
+      <x:c r="F17" s="1" t="s">
+        <x:v>243</x:v>
+      </x:c>
+      <x:c r="G17" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H17" s="1" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I17" s="1" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="A18" s="1" t="s">
         <x:v>129</x:v>
       </x:c>
       <x:c r="B18" s="1" t="s">
-        <x:v>259</x:v>
+        <x:v>260</x:v>
       </x:c>
       <x:c r="C18" s="1" t="s">
-        <x:v>292</x:v>
+        <x:v>293</x:v>
       </x:c>
       <x:c r="D18" s="1" t="s">
-        <x:v>270</x:v>
+        <x:v>271</x:v>
       </x:c>
       <x:c r="E18" s="1" t="s">
-        <x:v>290</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <x:v>291</x:v>
+      </x:c>
+      <x:c r="F18" s="1" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="G18" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H18" s="1" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I18" s="1" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="C19" s="7" t="s"/>
       <x:c r="E19" s="7" t="s"/>
     </x:row>
-    <x:row r="20" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <x:row r="20" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <x:c r="C20" s="7" t="s"/>
       <x:c r="E20" s="7" t="s"/>
     </x:row>
-    <x:row r="28" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <x:row r="33" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <x:row r="34" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <x:row r="28" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <x:row r="33" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <x:row r="34" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3836,8 +4055,527 @@
     <x:col min="12" max="13" width="11.632812" style="0" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
+    <x:row r="1" spans="1:13">
+      <x:c r="A1" s="0" t="s">
+        <x:v>251</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>252</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>253</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>254</x:v>
+      </x:c>
+      <x:c r="F1" s="0" t="s">
+        <x:v>255</x:v>
+      </x:c>
+      <x:c r="G1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="H1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="I1" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
     <x:row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <x:c r="E2" s="7" t="s"/>
+      <x:c r="A2" s="0" t="s">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>256</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>257</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>258</x:v>
+      </x:c>
+      <x:c r="E2" s="7" t="s">
+        <x:v>259</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="G2" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H2" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I2" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:13">
+      <x:c r="A3" s="0" t="s">
+        <x:v>135</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>261</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>262</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>261</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>134</x:v>
+      </x:c>
+      <x:c r="G3" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H3" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I3" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:13">
+      <x:c r="A4" s="0" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>256</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>263</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>264</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>265</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="G4" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H4" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I4" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:13">
+      <x:c r="A5" s="0" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>256</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>266</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>264</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>267</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="G5" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H5" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I5" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:13">
+      <x:c r="A6" s="0" t="s">
+        <x:v>98</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>256</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>268</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>264</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>269</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="G6" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H6" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I6" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:13">
+      <x:c r="A7" s="0" t="s">
+        <x:v>174</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>270</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>271</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>272</x:v>
+      </x:c>
+      <x:c r="F7" s="0" t="s">
+        <x:v>173</x:v>
+      </x:c>
+      <x:c r="G7" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H7" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I7" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:13">
+      <x:c r="A8" s="0" t="s">
+        <x:v>158</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>273</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>274</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="s">
+        <x:v>275</x:v>
+      </x:c>
+      <x:c r="F8" s="0" t="s">
+        <x:v>157</x:v>
+      </x:c>
+      <x:c r="G8" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H8" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I8" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:13">
+      <x:c r="A9" s="0" t="s">
+        <x:v>217</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>276</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>274</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="s">
+        <x:v>277</x:v>
+      </x:c>
+      <x:c r="F9" s="0" t="s">
+        <x:v>216</x:v>
+      </x:c>
+      <x:c r="G9" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H9" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I9" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:13">
+      <x:c r="A10" s="0" t="s">
+        <x:v>230</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>278</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>279</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="s">
+        <x:v>280</x:v>
+      </x:c>
+      <x:c r="F10" s="0" t="s">
+        <x:v>229</x:v>
+      </x:c>
+      <x:c r="G10" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H10" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I10" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:13">
+      <x:c r="A11" s="0" t="s">
+        <x:v>164</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>281</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>282</x:v>
+      </x:c>
+      <x:c r="E11" s="0" t="s">
+        <x:v>276</x:v>
+      </x:c>
+      <x:c r="F11" s="0" t="s">
+        <x:v>163</x:v>
+      </x:c>
+      <x:c r="G11" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H11" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I11" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:13">
+      <x:c r="A12" s="0" t="s">
+        <x:v>226</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
+        <x:v>283</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>282</x:v>
+      </x:c>
+      <x:c r="E12" s="0" t="s">
+        <x:v>284</x:v>
+      </x:c>
+      <x:c r="F12" s="0" t="s">
+        <x:v>225</x:v>
+      </x:c>
+      <x:c r="G12" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H12" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I12" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:13">
+      <x:c r="A13" s="0" t="s">
+        <x:v>155</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="s">
+        <x:v>285</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
+        <x:v>286</x:v>
+      </x:c>
+      <x:c r="E13" s="0" t="s">
+        <x:v>287</x:v>
+      </x:c>
+      <x:c r="F13" s="0" t="s">
+        <x:v>154</x:v>
+      </x:c>
+      <x:c r="G13" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H13" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I13" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:13">
+      <x:c r="A14" s="0" t="s">
+        <x:v>176</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
+        <x:v>288</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="s">
+        <x:v>289</x:v>
+      </x:c>
+      <x:c r="E14" s="0" t="s">
+        <x:v>290</x:v>
+      </x:c>
+      <x:c r="F14" s="0" t="s">
+        <x:v>175</x:v>
+      </x:c>
+      <x:c r="G14" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H14" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I14" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:13">
+      <x:c r="A15" s="0" t="s">
+        <x:v>144</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
+        <x:v>291</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="s">
+        <x:v>262</x:v>
+      </x:c>
+      <x:c r="E15" s="0" t="s">
+        <x:v>291</x:v>
+      </x:c>
+      <x:c r="F15" s="0" t="s">
+        <x:v>143</x:v>
+      </x:c>
+      <x:c r="G15" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H15" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I15" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:13">
+      <x:c r="A16" s="0" t="s">
+        <x:v>202</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>272</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
+        <x:v>262</x:v>
+      </x:c>
+      <x:c r="E16" s="0" t="s">
+        <x:v>272</x:v>
+      </x:c>
+      <x:c r="F16" s="0" t="s">
+        <x:v>201</x:v>
+      </x:c>
+      <x:c r="G16" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H16" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I16" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:13">
+      <x:c r="A17" s="0" t="s">
+        <x:v>244</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="s">
+        <x:v>292</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="s">
+        <x:v>262</x:v>
+      </x:c>
+      <x:c r="E17" s="0" t="s">
+        <x:v>292</x:v>
+      </x:c>
+      <x:c r="F17" s="0" t="s">
+        <x:v>243</x:v>
+      </x:c>
+      <x:c r="G17" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H17" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I17" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:13">
+      <x:c r="A18" s="0" t="s">
+        <x:v>129</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
+        <x:v>260</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="s">
+        <x:v>293</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="s">
+        <x:v>271</x:v>
+      </x:c>
+      <x:c r="E18" s="0" t="s">
+        <x:v>291</x:v>
+      </x:c>
+      <x:c r="F18" s="0" t="s">
+        <x:v>128</x:v>
+      </x:c>
+      <x:c r="G18" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H18" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I18" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>